<commit_message>
add more student data
</commit_message>
<xml_diff>
--- a/data/student_data.xlsx
+++ b/data/student_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05DD7FA-6D55-4287-9A05-0E9386AE3E5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621C9F8D-3CCC-4FB8-9C5B-74FD09887E42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>fname</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t>222-00-2222</t>
+  </si>
+  <si>
+    <t>Barney</t>
+  </si>
+  <si>
+    <t>Fife</t>
+  </si>
+  <si>
+    <t>333-11-2345</t>
   </si>
 </sst>
 </file>
@@ -364,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,6 +417,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "add more student data"
This reverts commit 8cc7cfd2512fa7f6ab2208a31774a79dc7076926.
</commit_message>
<xml_diff>
--- a/data/student_data.xlsx
+++ b/data/student_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621C9F8D-3CCC-4FB8-9C5B-74FD09887E42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05DD7FA-6D55-4287-9A05-0E9386AE3E5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>fname</t>
   </si>
@@ -47,15 +47,6 @@
   </si>
   <si>
     <t>222-00-2222</t>
-  </si>
-  <si>
-    <t>Barney</t>
-  </si>
-  <si>
-    <t>Fife</t>
-  </si>
-  <si>
-    <t>333-11-2345</t>
   </si>
 </sst>
 </file>
@@ -373,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,17 +408,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>